<commit_message>
Updated many items overall revamp
</commit_message>
<xml_diff>
--- a/OrganicChemistryBoardGame.xlsx
+++ b/OrganicChemistryBoardGame.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Barry\Organic Chemistry Board Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D87DFA-DB34-4D04-9EE1-7E8E8E7FCF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044F1C10-3D50-4693-BCB8-62500F62833E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1930,21 +1930,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C194" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E205" sqref="E205"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>313</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>88</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>90</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>93</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>94</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>95</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>101</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>102</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>264</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>265</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>266</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>267</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>106</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>268</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>108</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>110</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>111</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>269</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>112</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>270</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>271</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>272</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>273</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>274</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>275</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>276</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>277</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>278</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>279</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>280</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>281</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>282</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>283</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>284</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>285</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>286</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>113</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>114</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>288</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>115</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>116</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>117</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>289</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>118</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>287</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>290</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>119</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>291</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>292</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>293</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>120</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>121</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>122</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>123</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>124</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>294</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>295</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>125</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>126</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>127</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>128</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>296</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>129</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>130</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>297</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>131</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>132</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>133</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>134</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>135</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>136</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>298</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>137</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>138</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>139</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>140</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>309</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>300</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>301</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>311</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>95</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>236</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>237</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>238</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>239</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>240</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>241</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>242</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>243</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>244</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>245</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>246</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>247</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>248</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>249</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>250</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>251</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>252</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>253</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>254</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>255</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>256</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>257</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>258</v>
       </c>
@@ -5379,7 +5379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>259</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>260</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>302</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>305</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C154" t="s">
         <v>467</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C155" t="s">
         <v>468</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C156" t="s">
         <v>469</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C157" t="s">
         <v>470</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C158" t="s">
         <v>471</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C159" t="s">
         <v>472</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C160" t="s">
         <v>473</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C161" t="s">
         <v>474</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C162" t="s">
         <v>475</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C163" t="s">
         <v>476</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C164" t="s">
         <v>477</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C165" t="s">
         <v>478</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C166" t="s">
         <v>479</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C167" t="s">
         <v>480</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C168" t="s">
         <v>481</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C169" t="s">
         <v>482</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C170" t="s">
         <v>483</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C171" t="s">
         <v>484</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C172" t="s">
         <v>485</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C173" t="s">
         <v>486</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C174" t="s">
         <v>487</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C175" t="s">
         <v>488</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C176" t="s">
         <v>489</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C177" t="s">
         <v>490</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C178" t="s">
         <v>491</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C179" t="s">
         <v>492</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C180" t="s">
         <v>493</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C181" t="s">
         <v>494</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C182" t="s">
         <v>495</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C183" t="s">
         <v>496</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C184" t="s">
         <v>497</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C185" t="s">
         <v>498</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C186" t="s">
         <v>499</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C187" t="s">
         <v>500</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C188" t="s">
         <v>501</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C189" t="s">
         <v>502</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C190" t="s">
         <v>503</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C191" t="s">
         <v>504</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C192" t="s">
         <v>505</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C193" t="s">
         <v>506</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C194" t="s">
         <v>507</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C195" t="s">
         <v>508</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C196" t="s">
         <v>509</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C197" t="s">
         <v>510</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C198" t="s">
         <v>511</v>
       </c>
@@ -6236,7 +6236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C199" t="s">
         <v>512</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C200" t="s">
         <v>513</v>
       </c>
@@ -6270,7 +6270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:9" x14ac:dyDescent="0.45">
       <c r="E201" t="s">
         <v>519</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="202" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:9" x14ac:dyDescent="0.45">
       <c r="E202" t="s">
         <v>520</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>40.555555555555557</v>
       </c>
     </row>
-    <row r="203" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:9" x14ac:dyDescent="0.45">
       <c r="E203" t="s">
         <v>521</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:9" x14ac:dyDescent="0.45">
       <c r="E204" t="s">
         <v>522</v>
       </c>

</xml_diff>